<commit_message>
split the crude oil cells into another location within the spreadsheet
</commit_message>
<xml_diff>
--- a/etl_processor/data_source/energy/TotalFinalEnergyConsumptionByEnergyTypeAndSector.xlsx
+++ b/etl_processor/data_source/energy/TotalFinalEnergyConsumptionByEnergyTypeAndSector.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10714"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB11A39-9BEB-6340-81EB-CADB95D8CEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E70A699-709F-D445-B89B-B3232FE62310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="47">
   <si>
     <t/>
   </si>
@@ -570,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N143"/>
+  <dimension ref="A1:N131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2662,90 +2662,90 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B80" s="5">
-        <v>184.6</v>
-      </c>
-      <c r="C80" s="5">
-        <v>182.7</v>
-      </c>
-      <c r="D80" s="5">
-        <v>180.9</v>
-      </c>
-      <c r="E80" s="5">
-        <v>182.5</v>
-      </c>
-      <c r="F80" s="5">
-        <v>600.5</v>
-      </c>
-      <c r="G80" s="5">
-        <v>166.8</v>
-      </c>
-      <c r="H80" s="5">
-        <v>162.9</v>
-      </c>
-      <c r="I80" s="5">
-        <v>162.19999999999999</v>
-      </c>
-      <c r="J80" s="6">
-        <v>129</v>
-      </c>
-      <c r="K80" s="6">
-        <v>23</v>
-      </c>
-      <c r="L80" s="5">
-        <v>5.7</v>
-      </c>
-      <c r="M80" s="5">
-        <v>5.9</v>
-      </c>
-      <c r="N80" s="6">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I80" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J80" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K80" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L80" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M80" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N80" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B81" s="5">
-        <v>184.6</v>
-      </c>
-      <c r="C81" s="5">
-        <v>182.7</v>
-      </c>
-      <c r="D81" s="5">
-        <v>180.9</v>
-      </c>
-      <c r="E81" s="5">
-        <v>182.5</v>
-      </c>
-      <c r="F81" s="5">
-        <v>600.5</v>
-      </c>
-      <c r="G81" s="5">
-        <v>166.8</v>
-      </c>
-      <c r="H81" s="5">
-        <v>162.9</v>
-      </c>
-      <c r="I81" s="5">
-        <v>162.19999999999999</v>
-      </c>
-      <c r="J81" s="6">
-        <v>129</v>
-      </c>
-      <c r="K81" s="6">
-        <v>23</v>
-      </c>
-      <c r="L81" s="5">
-        <v>5.7</v>
-      </c>
-      <c r="M81" s="5">
-        <v>5.9</v>
-      </c>
-      <c r="N81" s="6">
-        <v>3</v>
+      <c r="B81" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H81" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I81" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J81" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K81" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L81" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M81" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N81" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
@@ -2924,1763 +2924,1235 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A86" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G86" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H86" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I86" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J86" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K86" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L86" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M86" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N86" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A87" s="4" t="s">
+    <row r="92" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J92" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K92" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L92" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M92" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N92" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B93" s="5">
+        <v>9009.4</v>
+      </c>
+      <c r="C93" s="5">
+        <v>8713.2999999999993</v>
+      </c>
+      <c r="D93" s="5">
+        <v>10125.1</v>
+      </c>
+      <c r="E93" s="5">
+        <v>9073.5</v>
+      </c>
+      <c r="F93" s="5">
+        <v>9149.5</v>
+      </c>
+      <c r="G93" s="5">
+        <v>9351.2000000000007</v>
+      </c>
+      <c r="H93" s="5">
+        <v>9993.4</v>
+      </c>
+      <c r="I93" s="5">
+        <v>8968.2999999999993</v>
+      </c>
+      <c r="J93" s="6">
+        <v>8475</v>
+      </c>
+      <c r="K93" s="5">
+        <v>7946.8</v>
+      </c>
+      <c r="L93" s="6">
+        <v>7614</v>
+      </c>
+      <c r="M93" s="5">
+        <v>7790.2</v>
+      </c>
+      <c r="N93" s="5">
+        <v>6474.8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B87" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G87" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H87" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I87" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J87" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K87" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L87" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M87" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N87" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A88" s="4" t="s">
+      <c r="B94" s="5">
+        <v>6423.7</v>
+      </c>
+      <c r="C94" s="5">
+        <v>6406.7</v>
+      </c>
+      <c r="D94" s="5">
+        <v>7611.1</v>
+      </c>
+      <c r="E94" s="5">
+        <v>6519.2</v>
+      </c>
+      <c r="F94" s="5">
+        <v>6562.8</v>
+      </c>
+      <c r="G94" s="5">
+        <v>6567.2</v>
+      </c>
+      <c r="H94" s="5">
+        <v>7265.1</v>
+      </c>
+      <c r="I94" s="5">
+        <v>6665.5</v>
+      </c>
+      <c r="J94" s="5">
+        <v>6225.3</v>
+      </c>
+      <c r="K94" s="6">
+        <v>5562</v>
+      </c>
+      <c r="L94" s="5">
+        <v>5153.3999999999996</v>
+      </c>
+      <c r="M94" s="5">
+        <v>5465.2</v>
+      </c>
+      <c r="N94" s="5">
+        <v>4177.7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B88" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G88" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H88" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I88" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J88" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K88" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L88" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M88" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N88" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A89" s="4" t="s">
+      <c r="B95" s="5">
+        <v>75.2</v>
+      </c>
+      <c r="C95" s="5">
+        <v>69.3</v>
+      </c>
+      <c r="D95" s="5">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="E95" s="5">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="F95" s="5">
+        <v>75.2</v>
+      </c>
+      <c r="G95" s="5">
+        <v>77.3</v>
+      </c>
+      <c r="H95" s="6">
+        <v>80</v>
+      </c>
+      <c r="I95" s="5">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="J95" s="5">
+        <v>87.3</v>
+      </c>
+      <c r="K95" s="5">
+        <v>68.3</v>
+      </c>
+      <c r="L95" s="5">
+        <v>68.900000000000006</v>
+      </c>
+      <c r="M95" s="5">
+        <v>84.2</v>
+      </c>
+      <c r="N95" s="5">
+        <v>78.5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B89" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C89" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G89" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H89" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I89" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J89" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K89" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L89" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M89" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N89" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A90" s="4" t="s">
+      <c r="B96" s="5">
+        <v>2485.5</v>
+      </c>
+      <c r="C96" s="5">
+        <v>2214.3000000000002</v>
+      </c>
+      <c r="D96" s="5">
+        <v>2420.1999999999998</v>
+      </c>
+      <c r="E96" s="5">
+        <v>2455.1</v>
+      </c>
+      <c r="F96" s="5">
+        <v>2486.5</v>
+      </c>
+      <c r="G96" s="5">
+        <v>2680.9</v>
+      </c>
+      <c r="H96" s="5">
+        <v>2621.5</v>
+      </c>
+      <c r="I96" s="5">
+        <v>2199.8000000000002</v>
+      </c>
+      <c r="J96" s="5">
+        <v>2133.3000000000002</v>
+      </c>
+      <c r="K96" s="5">
+        <v>2292.6999999999998</v>
+      </c>
+      <c r="L96" s="5">
+        <v>2366.9</v>
+      </c>
+      <c r="M96" s="5">
+        <v>2219.1</v>
+      </c>
+      <c r="N96" s="5">
+        <v>2193.3000000000002</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A97" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B90" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C90" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G90" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H90" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I90" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J90" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K90" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L90" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M90" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N90" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A91" s="4" t="s">
+      <c r="B97" s="5">
+        <v>25.1</v>
+      </c>
+      <c r="C97" s="5">
+        <v>23.1</v>
+      </c>
+      <c r="D97" s="5">
+        <v>23.5</v>
+      </c>
+      <c r="E97" s="5">
+        <v>24.8</v>
+      </c>
+      <c r="F97" s="5">
+        <v>25.1</v>
+      </c>
+      <c r="G97" s="5">
+        <v>25.8</v>
+      </c>
+      <c r="H97" s="5">
+        <v>26.7</v>
+      </c>
+      <c r="I97" s="5">
+        <v>24.1</v>
+      </c>
+      <c r="J97" s="5">
+        <v>29.1</v>
+      </c>
+      <c r="K97" s="5">
+        <v>23.7</v>
+      </c>
+      <c r="L97" s="5">
+        <v>24.8</v>
+      </c>
+      <c r="M97" s="5">
+        <v>21.7</v>
+      </c>
+      <c r="N97" s="5">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A98" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B91" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G91" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H91" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I91" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J91" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K91" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L91" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M91" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N91" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A98" s="3" t="s">
+      <c r="B98" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H98" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I98" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J98" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K98" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L98" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M98" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N98" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B101" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="C101" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D98" s="3" t="s">
+      <c r="D101" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E98" s="3" t="s">
+      <c r="E101" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F98" s="3" t="s">
+      <c r="F101" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G98" s="3" t="s">
+      <c r="G101" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H98" s="3" t="s">
+      <c r="H101" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I98" s="3" t="s">
+      <c r="I101" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J98" s="3" t="s">
+      <c r="J101" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K98" s="3" t="s">
+      <c r="K101" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L98" s="3" t="s">
+      <c r="L101" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M98" s="3" t="s">
+      <c r="M101" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N98" s="3" t="s">
+      <c r="N101" s="3" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A99" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B99" s="5">
-        <v>9009.4</v>
-      </c>
-      <c r="C99" s="5">
-        <v>8713.2999999999993</v>
-      </c>
-      <c r="D99" s="5">
-        <v>10125.1</v>
-      </c>
-      <c r="E99" s="5">
-        <v>9073.5</v>
-      </c>
-      <c r="F99" s="5">
-        <v>9149.5</v>
-      </c>
-      <c r="G99" s="5">
-        <v>9351.2000000000007</v>
-      </c>
-      <c r="H99" s="5">
-        <v>9993.4</v>
-      </c>
-      <c r="I99" s="5">
-        <v>8968.2999999999993</v>
-      </c>
-      <c r="J99" s="6">
-        <v>8475</v>
-      </c>
-      <c r="K99" s="5">
-        <v>7946.8</v>
-      </c>
-      <c r="L99" s="6">
-        <v>7614</v>
-      </c>
-      <c r="M99" s="5">
-        <v>7790.2</v>
-      </c>
-      <c r="N99" s="5">
-        <v>6474.8</v>
-      </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A100" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B100" s="5">
-        <v>6423.7</v>
-      </c>
-      <c r="C100" s="5">
-        <v>6406.7</v>
-      </c>
-      <c r="D100" s="5">
-        <v>7611.1</v>
-      </c>
-      <c r="E100" s="5">
-        <v>6519.2</v>
-      </c>
-      <c r="F100" s="5">
-        <v>6562.8</v>
-      </c>
-      <c r="G100" s="5">
-        <v>6567.2</v>
-      </c>
-      <c r="H100" s="5">
-        <v>7265.1</v>
-      </c>
-      <c r="I100" s="5">
-        <v>6665.5</v>
-      </c>
-      <c r="J100" s="5">
-        <v>6225.3</v>
-      </c>
-      <c r="K100" s="6">
-        <v>5562</v>
-      </c>
-      <c r="L100" s="5">
-        <v>5153.3999999999996</v>
-      </c>
-      <c r="M100" s="5">
-        <v>5465.2</v>
-      </c>
-      <c r="N100" s="5">
-        <v>4177.7</v>
-      </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A101" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B101" s="5">
-        <v>75.2</v>
-      </c>
-      <c r="C101" s="5">
-        <v>69.3</v>
-      </c>
-      <c r="D101" s="5">
-        <v>70.400000000000006</v>
-      </c>
-      <c r="E101" s="5">
-        <v>74.400000000000006</v>
-      </c>
-      <c r="F101" s="5">
-        <v>75.2</v>
-      </c>
-      <c r="G101" s="5">
-        <v>77.3</v>
-      </c>
-      <c r="H101" s="6">
-        <v>80</v>
-      </c>
-      <c r="I101" s="5">
-        <v>78.900000000000006</v>
-      </c>
-      <c r="J101" s="5">
-        <v>87.3</v>
-      </c>
-      <c r="K101" s="5">
-        <v>68.3</v>
-      </c>
-      <c r="L101" s="5">
-        <v>68.900000000000006</v>
-      </c>
-      <c r="M101" s="5">
-        <v>84.2</v>
-      </c>
-      <c r="N101" s="5">
-        <v>78.5</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B102" s="5">
-        <v>2485.5</v>
+        <v>184.6</v>
       </c>
       <c r="C102" s="5">
-        <v>2214.3000000000002</v>
+        <v>182.7</v>
       </c>
       <c r="D102" s="5">
-        <v>2420.1999999999998</v>
+        <v>180.9</v>
       </c>
       <c r="E102" s="5">
-        <v>2455.1</v>
+        <v>182.5</v>
       </c>
       <c r="F102" s="5">
-        <v>2486.5</v>
+        <v>600.5</v>
       </c>
       <c r="G102" s="5">
-        <v>2680.9</v>
+        <v>166.8</v>
       </c>
       <c r="H102" s="5">
-        <v>2621.5</v>
+        <v>162.9</v>
       </c>
       <c r="I102" s="5">
-        <v>2199.8000000000002</v>
-      </c>
-      <c r="J102" s="5">
-        <v>2133.3000000000002</v>
-      </c>
-      <c r="K102" s="5">
-        <v>2292.6999999999998</v>
+        <v>162.19999999999999</v>
+      </c>
+      <c r="J102" s="6">
+        <v>129</v>
+      </c>
+      <c r="K102" s="6">
+        <v>23</v>
       </c>
       <c r="L102" s="5">
-        <v>2366.9</v>
+        <v>5.7</v>
       </c>
       <c r="M102" s="5">
-        <v>2219.1</v>
-      </c>
-      <c r="N102" s="5">
-        <v>2193.3000000000002</v>
+        <v>5.9</v>
+      </c>
+      <c r="N102" s="6">
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B103" s="5">
-        <v>25.1</v>
+        <v>184.6</v>
       </c>
       <c r="C103" s="5">
-        <v>23.1</v>
+        <v>182.7</v>
       </c>
       <c r="D103" s="5">
-        <v>23.5</v>
+        <v>180.9</v>
       </c>
       <c r="E103" s="5">
-        <v>24.8</v>
+        <v>182.5</v>
       </c>
       <c r="F103" s="5">
-        <v>25.1</v>
+        <v>600.5</v>
       </c>
       <c r="G103" s="5">
-        <v>25.8</v>
+        <v>166.8</v>
       </c>
       <c r="H103" s="5">
-        <v>26.7</v>
+        <v>162.9</v>
       </c>
       <c r="I103" s="5">
-        <v>24.1</v>
-      </c>
-      <c r="J103" s="5">
-        <v>29.1</v>
-      </c>
-      <c r="K103" s="5">
-        <v>23.7</v>
+        <v>162.19999999999999</v>
+      </c>
+      <c r="J103" s="6">
+        <v>129</v>
+      </c>
+      <c r="K103" s="6">
+        <v>23</v>
       </c>
       <c r="L103" s="5">
-        <v>24.8</v>
+        <v>5.7</v>
       </c>
       <c r="M103" s="5">
-        <v>21.7</v>
-      </c>
-      <c r="N103" s="5">
-        <v>25.3</v>
+        <v>5.9</v>
+      </c>
+      <c r="N103" s="6">
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N104" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A105" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G105" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H105" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I105" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J105" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K105" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L105" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M105" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N105" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A106" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N106" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A107" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B104" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C104" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D104" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E104" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F104" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G104" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H104" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I104" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J104" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K104" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L104" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M104" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N104" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="107" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A107" s="3" t="s">
+      <c r="B107" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G107" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H107" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I107" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J107" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K107" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L107" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M107" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N107" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B115" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="C115" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D107" s="3" t="s">
+      <c r="D115" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E107" s="3" t="s">
+      <c r="E115" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F107" s="3" t="s">
+      <c r="F115" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G107" s="3" t="s">
+      <c r="G115" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H107" s="3" t="s">
+      <c r="H115" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I107" s="3" t="s">
+      <c r="I115" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J107" s="3" t="s">
+      <c r="J115" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K107" s="3" t="s">
+      <c r="K115" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L107" s="3" t="s">
+      <c r="L115" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M107" s="3" t="s">
+      <c r="M115" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N107" s="3" t="s">
+      <c r="N115" s="3" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A108" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B108" s="5">
-        <v>15534.2</v>
-      </c>
-      <c r="C108" s="5">
-        <v>14900.6</v>
-      </c>
-      <c r="D108" s="5">
-        <v>16236.3</v>
-      </c>
-      <c r="E108" s="5">
-        <v>15074.3</v>
-      </c>
-      <c r="F108" s="5">
-        <v>15456.6</v>
-      </c>
-      <c r="G108" s="6">
-        <v>15059</v>
-      </c>
-      <c r="H108" s="5">
-        <v>15582.2</v>
-      </c>
-      <c r="I108" s="5">
-        <v>14475.5</v>
-      </c>
-      <c r="J108" s="5">
-        <v>13780.5</v>
-      </c>
-      <c r="K108" s="5">
-        <v>12896.5</v>
-      </c>
-      <c r="L108" s="5">
-        <v>12501.6</v>
-      </c>
-      <c r="M108" s="5">
-        <v>12557.5</v>
-      </c>
-      <c r="N108" s="5">
-        <v>10683.8</v>
-      </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A109" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B109" s="5">
-        <v>10087.799999999999</v>
-      </c>
-      <c r="C109" s="5">
-        <v>9872.7999999999993</v>
-      </c>
-      <c r="D109" s="5">
-        <v>10962.6</v>
-      </c>
-      <c r="E109" s="5">
-        <v>9866.6</v>
-      </c>
-      <c r="F109" s="5">
-        <v>10268.1</v>
-      </c>
-      <c r="G109" s="5">
-        <v>9683.1</v>
-      </c>
-      <c r="H109" s="5">
-        <v>10331.4</v>
-      </c>
-      <c r="I109" s="5">
-        <v>9718.9</v>
-      </c>
-      <c r="J109" s="5">
-        <v>9120.4</v>
-      </c>
-      <c r="K109" s="6">
-        <v>8148</v>
-      </c>
-      <c r="L109" s="5">
-        <v>7733.2</v>
-      </c>
-      <c r="M109" s="5">
-        <v>7964.4</v>
-      </c>
-      <c r="N109" s="5">
-        <v>6245.9</v>
-      </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A110" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B110" s="5">
-        <v>1881.4</v>
-      </c>
-      <c r="C110" s="6">
-        <v>1739</v>
-      </c>
-      <c r="D110" s="5">
-        <v>1819.3</v>
-      </c>
-      <c r="E110" s="6">
-        <v>1760</v>
-      </c>
-      <c r="F110" s="5">
-        <v>1716.6</v>
-      </c>
-      <c r="G110" s="5">
-        <v>1691.3</v>
-      </c>
-      <c r="H110" s="5">
-        <v>1671.3</v>
-      </c>
-      <c r="I110" s="5">
-        <v>1629.8</v>
-      </c>
-      <c r="J110" s="5">
-        <v>1614.2</v>
-      </c>
-      <c r="K110" s="6">
-        <v>1558</v>
-      </c>
-      <c r="L110" s="5">
-        <v>1516.4</v>
-      </c>
-      <c r="M110" s="5">
-        <v>1492.6</v>
-      </c>
-      <c r="N110" s="5">
-        <v>1423.9</v>
-      </c>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A111" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B111" s="5">
-        <v>2733.2</v>
-      </c>
-      <c r="C111" s="5">
-        <v>2457.8000000000002</v>
-      </c>
-      <c r="D111" s="5">
-        <v>2682.5</v>
-      </c>
-      <c r="E111" s="5">
-        <v>2711.4</v>
-      </c>
-      <c r="F111" s="5">
-        <v>2731.7</v>
-      </c>
-      <c r="G111" s="6">
-        <v>2919</v>
-      </c>
-      <c r="H111" s="6">
-        <v>2846</v>
-      </c>
-      <c r="I111" s="6">
-        <v>2427</v>
-      </c>
-      <c r="J111" s="5">
-        <v>2355.1</v>
-      </c>
-      <c r="K111" s="5">
-        <v>2512.9</v>
-      </c>
-      <c r="L111" s="5">
-        <v>2584.1</v>
-      </c>
-      <c r="M111" s="5">
-        <v>2420.4</v>
-      </c>
-      <c r="N111" s="5">
-        <v>2345.3000000000002</v>
-      </c>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A112" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B112" s="5">
-        <v>808.9</v>
-      </c>
-      <c r="C112" s="5">
-        <v>808.2</v>
-      </c>
-      <c r="D112" s="5">
-        <v>747.2</v>
-      </c>
-      <c r="E112" s="5">
-        <v>710.3</v>
-      </c>
-      <c r="F112" s="5">
-        <v>714.1</v>
-      </c>
-      <c r="G112" s="5">
-        <v>738.9</v>
-      </c>
-      <c r="H112" s="5">
-        <v>707.5</v>
-      </c>
-      <c r="I112" s="5">
-        <v>678.4</v>
-      </c>
-      <c r="J112" s="5">
-        <v>667.5</v>
-      </c>
-      <c r="K112" s="5">
-        <v>650.70000000000005</v>
-      </c>
-      <c r="L112" s="5">
-        <v>637.4</v>
-      </c>
-      <c r="M112" s="5">
-        <v>646.20000000000005</v>
-      </c>
-      <c r="N112" s="5">
-        <v>632.29999999999995</v>
-      </c>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A113" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B113" s="5">
-        <v>22.9</v>
-      </c>
-      <c r="C113" s="5">
-        <v>22.8</v>
-      </c>
-      <c r="D113" s="5">
-        <v>24.8</v>
-      </c>
-      <c r="E113" s="5">
-        <v>26.1</v>
-      </c>
-      <c r="F113" s="5">
-        <v>26.2</v>
-      </c>
-      <c r="G113" s="5">
-        <v>26.7</v>
-      </c>
-      <c r="H113" s="6">
-        <v>26</v>
-      </c>
-      <c r="I113" s="5">
-        <v>21.3</v>
-      </c>
-      <c r="J113" s="5">
-        <v>23.4</v>
-      </c>
-      <c r="K113" s="5">
-        <v>26.9</v>
-      </c>
-      <c r="L113" s="5">
-        <v>30.6</v>
-      </c>
-      <c r="M113" s="5">
-        <v>33.9</v>
-      </c>
-      <c r="N113" s="5">
-        <v>36.4</v>
-      </c>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A114" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B114" s="5">
-        <v>184.6</v>
-      </c>
-      <c r="C114" s="5">
-        <v>182.7</v>
-      </c>
-      <c r="D114" s="5">
-        <v>180.9</v>
-      </c>
-      <c r="E114" s="5">
-        <v>182.5</v>
-      </c>
-      <c r="F114" s="5">
-        <v>600.5</v>
-      </c>
-      <c r="G114" s="5">
-        <v>166.8</v>
-      </c>
-      <c r="H114" s="5">
-        <v>162.9</v>
-      </c>
-      <c r="I114" s="5">
-        <v>162.19999999999999</v>
-      </c>
-      <c r="J114" s="6">
-        <v>129</v>
-      </c>
-      <c r="K114" s="6">
-        <v>23</v>
-      </c>
-      <c r="L114" s="5">
-        <v>5.7</v>
-      </c>
-      <c r="M114" s="5">
-        <v>5.9</v>
-      </c>
-      <c r="N114" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A115" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B115" s="5">
-        <v>184.6</v>
-      </c>
-      <c r="C115" s="5">
-        <v>182.7</v>
-      </c>
-      <c r="D115" s="5">
-        <v>180.9</v>
-      </c>
-      <c r="E115" s="5">
-        <v>182.5</v>
-      </c>
-      <c r="F115" s="5">
-        <v>600.5</v>
-      </c>
-      <c r="G115" s="5">
-        <v>166.8</v>
-      </c>
-      <c r="H115" s="5">
-        <v>162.9</v>
-      </c>
-      <c r="I115" s="5">
-        <v>162.19999999999999</v>
-      </c>
-      <c r="J115" s="6">
-        <v>129</v>
-      </c>
-      <c r="K115" s="6">
-        <v>23</v>
-      </c>
-      <c r="L115" s="5">
-        <v>5.7</v>
-      </c>
-      <c r="M115" s="5">
-        <v>5.9</v>
-      </c>
-      <c r="N115" s="6">
-        <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B116" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C116" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D116" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E116" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F116" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G116" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H116" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I116" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J116" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K116" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L116" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M116" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N116" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="B116" s="5">
+        <v>4598.7</v>
+      </c>
+      <c r="C116" s="5">
+        <v>4366.3</v>
+      </c>
+      <c r="D116" s="6">
+        <v>4448</v>
+      </c>
+      <c r="E116" s="5">
+        <v>4338.8999999999996</v>
+      </c>
+      <c r="F116" s="5">
+        <v>4268.1000000000004</v>
+      </c>
+      <c r="G116" s="5">
+        <v>4180.8</v>
+      </c>
+      <c r="H116" s="5">
+        <v>4085.5</v>
+      </c>
+      <c r="I116" s="5">
+        <v>3989.9</v>
+      </c>
+      <c r="J116" s="5">
+        <v>3864.9</v>
+      </c>
+      <c r="K116" s="5">
+        <v>3800.6</v>
+      </c>
+      <c r="L116" s="6">
+        <v>3698</v>
+      </c>
+      <c r="M116" s="6">
+        <v>3633</v>
+      </c>
+      <c r="N116" s="5">
+        <v>3338.2</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B117" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C117" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D117" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E117" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F117" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G117" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H117" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I117" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J117" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K117" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L117" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M117" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N117" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
+      </c>
+      <c r="B117" s="5">
+        <v>1916.9</v>
+      </c>
+      <c r="C117" s="5">
+        <v>1803.9</v>
+      </c>
+      <c r="D117" s="5">
+        <v>1845.6</v>
+      </c>
+      <c r="E117" s="5">
+        <v>1843.5</v>
+      </c>
+      <c r="F117" s="5">
+        <v>1826.3</v>
+      </c>
+      <c r="G117" s="5">
+        <v>1755.7</v>
+      </c>
+      <c r="H117" s="5">
+        <v>1727.3</v>
+      </c>
+      <c r="I117" s="5">
+        <v>1698.5</v>
+      </c>
+      <c r="J117" s="5">
+        <v>1620.2</v>
+      </c>
+      <c r="K117" s="6">
+        <v>1597</v>
+      </c>
+      <c r="L117" s="5">
+        <v>1554.4</v>
+      </c>
+      <c r="M117" s="5">
+        <v>1518.7</v>
+      </c>
+      <c r="N117" s="5">
+        <v>1338.8</v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B118" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C118" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D118" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E118" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F118" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G118" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H118" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I118" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J118" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K118" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L118" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M118" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N118" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
+      </c>
+      <c r="B118" s="5">
+        <v>1705.7</v>
+      </c>
+      <c r="C118" s="5">
+        <v>1592.2</v>
+      </c>
+      <c r="D118" s="5">
+        <v>1661.1</v>
+      </c>
+      <c r="E118" s="5">
+        <v>1597.9</v>
+      </c>
+      <c r="F118" s="5">
+        <v>1552.9</v>
+      </c>
+      <c r="G118" s="5">
+        <v>1521.9</v>
+      </c>
+      <c r="H118" s="5">
+        <v>1503.1</v>
+      </c>
+      <c r="I118" s="5">
+        <v>1465.7</v>
+      </c>
+      <c r="J118" s="5">
+        <v>1437.5</v>
+      </c>
+      <c r="K118" s="5">
+        <v>1407.2</v>
+      </c>
+      <c r="L118" s="5">
+        <v>1365.1</v>
+      </c>
+      <c r="M118" s="5">
+        <v>1330.2</v>
+      </c>
+      <c r="N118" s="5">
+        <v>1272.5999999999999</v>
       </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B119" s="5">
+        <v>244.6</v>
+      </c>
+      <c r="C119" s="5">
+        <v>241.5</v>
+      </c>
+      <c r="D119" s="5">
+        <v>259.60000000000002</v>
+      </c>
+      <c r="E119" s="5">
+        <v>253.4</v>
+      </c>
+      <c r="F119" s="5">
+        <v>238.3</v>
+      </c>
+      <c r="G119" s="5">
+        <v>226.9</v>
+      </c>
+      <c r="H119" s="5">
+        <v>210.2</v>
+      </c>
+      <c r="I119" s="5">
+        <v>209.9</v>
+      </c>
+      <c r="J119" s="5">
+        <v>203.7</v>
+      </c>
+      <c r="K119" s="5">
+        <v>200.2</v>
+      </c>
+      <c r="L119" s="5">
+        <v>191.2</v>
+      </c>
+      <c r="M119" s="5">
+        <v>180.5</v>
+      </c>
+      <c r="N119" s="5">
+        <v>138.19999999999999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A120" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B120" s="5">
+        <v>711.8</v>
+      </c>
+      <c r="C120" s="5">
+        <v>708.9</v>
+      </c>
+      <c r="D120" s="5">
+        <v>660.5</v>
+      </c>
+      <c r="E120" s="5">
+        <v>621.79999999999995</v>
+      </c>
+      <c r="F120" s="5">
+        <v>626.79999999999995</v>
+      </c>
+      <c r="G120" s="5">
+        <v>652.29999999999995</v>
+      </c>
+      <c r="H120" s="5">
+        <v>620.9</v>
+      </c>
+      <c r="I120" s="5">
+        <v>595.4</v>
+      </c>
+      <c r="J120" s="5">
+        <v>580.79999999999995</v>
+      </c>
+      <c r="K120" s="6">
+        <v>570</v>
+      </c>
+      <c r="L120" s="5">
+        <v>557.4</v>
+      </c>
+      <c r="M120" s="5">
+        <v>570.6</v>
+      </c>
+      <c r="N120" s="5">
+        <v>552.9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A121" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B119" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C119" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D119" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E119" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F119" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G119" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H119" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I119" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J119" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K119" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L119" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M119" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N119" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="127" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A127" s="3" t="s">
+      <c r="B121" s="5">
+        <v>19.8</v>
+      </c>
+      <c r="C121" s="5">
+        <v>19.7</v>
+      </c>
+      <c r="D121" s="5">
+        <v>21.2</v>
+      </c>
+      <c r="E121" s="5">
+        <v>22.2</v>
+      </c>
+      <c r="F121" s="5">
+        <v>23.8</v>
+      </c>
+      <c r="G121" s="5">
+        <v>24.1</v>
+      </c>
+      <c r="H121" s="6">
+        <v>24</v>
+      </c>
+      <c r="I121" s="5">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="J121" s="5">
+        <v>22.6</v>
+      </c>
+      <c r="K121" s="5">
+        <v>26.1</v>
+      </c>
+      <c r="L121" s="5">
+        <v>29.8</v>
+      </c>
+      <c r="M121" s="5">
+        <v>33.1</v>
+      </c>
+      <c r="N121" s="5">
+        <v>35.6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A125" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B127" s="3" t="s">
+      <c r="B125" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C127" s="3" t="s">
+      <c r="C125" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D127" s="3" t="s">
+      <c r="D125" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E127" s="3" t="s">
+      <c r="E125" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F127" s="3" t="s">
+      <c r="F125" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G127" s="3" t="s">
+      <c r="G125" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H127" s="3" t="s">
+      <c r="H125" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I127" s="3" t="s">
+      <c r="I125" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J127" s="3" t="s">
+      <c r="J125" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K127" s="3" t="s">
+      <c r="K125" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L127" s="3" t="s">
+      <c r="L125" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M127" s="3" t="s">
+      <c r="M125" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N127" s="3" t="s">
+      <c r="N125" s="3" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A126" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B126" s="5">
+        <v>1741.5</v>
+      </c>
+      <c r="C126" s="5">
+        <v>1638.3</v>
+      </c>
+      <c r="D126" s="5">
+        <v>1482.4</v>
+      </c>
+      <c r="E126" s="5">
+        <v>1479.5</v>
+      </c>
+      <c r="F126" s="5">
+        <v>1438.5</v>
+      </c>
+      <c r="G126" s="5">
+        <v>1360.2</v>
+      </c>
+      <c r="H126" s="5">
+        <v>1340.4</v>
+      </c>
+      <c r="I126" s="5">
+        <v>1355.1</v>
+      </c>
+      <c r="J126" s="5">
+        <v>1311.7</v>
+      </c>
+      <c r="K126" s="5">
+        <v>1126.2</v>
+      </c>
+      <c r="L126" s="5">
+        <v>1183.9000000000001</v>
+      </c>
+      <c r="M126" s="5">
+        <v>1128.4000000000001</v>
+      </c>
+      <c r="N126" s="5">
+        <v>867.9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A127" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B127" s="5">
+        <v>1562.7</v>
+      </c>
+      <c r="C127" s="5">
+        <v>1479.5</v>
+      </c>
+      <c r="D127" s="6">
+        <v>1325</v>
+      </c>
+      <c r="E127" s="5">
+        <v>1321.5</v>
+      </c>
+      <c r="F127" s="5">
+        <v>1278.4000000000001</v>
+      </c>
+      <c r="G127" s="5">
+        <v>1193.5</v>
+      </c>
+      <c r="H127" s="5">
+        <v>1176.0999999999999</v>
+      </c>
+      <c r="I127" s="5">
+        <v>1192.7</v>
+      </c>
+      <c r="J127" s="5">
+        <v>1145.9000000000001</v>
+      </c>
+      <c r="K127" s="6">
+        <v>966</v>
+      </c>
+      <c r="L127" s="5">
+        <v>1019.7</v>
+      </c>
+      <c r="M127" s="5">
+        <v>974.5</v>
+      </c>
+      <c r="N127" s="5">
+        <v>726.4</v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B128" s="5">
-        <v>4598.7</v>
+        <v>100.6</v>
       </c>
       <c r="C128" s="5">
-        <v>4366.3</v>
-      </c>
-      <c r="D128" s="6">
-        <v>4448</v>
+        <v>77.5</v>
+      </c>
+      <c r="D128" s="5">
+        <v>87.8</v>
       </c>
       <c r="E128" s="5">
-        <v>4338.8999999999996</v>
+        <v>87.6</v>
       </c>
       <c r="F128" s="5">
-        <v>4268.1000000000004</v>
+        <v>88.5</v>
       </c>
       <c r="G128" s="5">
-        <v>4180.8</v>
+        <v>92.1</v>
       </c>
       <c r="H128" s="5">
-        <v>4085.5</v>
+        <v>88.2</v>
       </c>
       <c r="I128" s="5">
-        <v>3989.9</v>
+        <v>85.3</v>
       </c>
       <c r="J128" s="5">
-        <v>3864.9</v>
+        <v>89.3</v>
       </c>
       <c r="K128" s="5">
-        <v>3800.6</v>
-      </c>
-      <c r="L128" s="6">
-        <v>3698</v>
-      </c>
-      <c r="M128" s="6">
-        <v>3633</v>
+        <v>82.5</v>
+      </c>
+      <c r="L128" s="5">
+        <v>82.4</v>
+      </c>
+      <c r="M128" s="5">
+        <v>78.3</v>
       </c>
       <c r="N128" s="5">
-        <v>3338.2</v>
+        <v>72.900000000000006</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B129" s="5">
-        <v>1916.9</v>
-      </c>
-      <c r="C129" s="5">
-        <v>1803.9</v>
+        <v>3.1</v>
+      </c>
+      <c r="C129" s="6">
+        <v>2</v>
       </c>
       <c r="D129" s="5">
-        <v>1845.6</v>
+        <v>2.7</v>
       </c>
       <c r="E129" s="5">
-        <v>1843.5</v>
+        <v>2.8</v>
       </c>
       <c r="F129" s="5">
-        <v>1826.3</v>
+        <v>6.9</v>
       </c>
       <c r="G129" s="5">
-        <v>1755.7</v>
+        <v>11.2</v>
       </c>
       <c r="H129" s="5">
-        <v>1727.3</v>
+        <v>14.3</v>
       </c>
       <c r="I129" s="5">
-        <v>1698.5</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="J129" s="5">
-        <v>1620.2</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="K129" s="6">
-        <v>1597</v>
+        <v>20</v>
       </c>
       <c r="L129" s="5">
-        <v>1554.4</v>
+        <v>25.9</v>
       </c>
       <c r="M129" s="5">
-        <v>1518.7</v>
+        <v>20.8</v>
       </c>
       <c r="N129" s="5">
-        <v>1338.8</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B130" s="5">
-        <v>1705.7</v>
+        <v>26</v>
+      </c>
+      <c r="B130" s="6">
+        <v>72</v>
       </c>
       <c r="C130" s="5">
-        <v>1592.2</v>
+        <v>76.2</v>
       </c>
       <c r="D130" s="5">
-        <v>1661.1</v>
+        <v>63.3</v>
       </c>
       <c r="E130" s="5">
-        <v>1597.9</v>
+        <v>63.7</v>
       </c>
       <c r="F130" s="5">
-        <v>1552.9</v>
+        <v>62.2</v>
       </c>
       <c r="G130" s="5">
-        <v>1521.9</v>
+        <v>60.9</v>
       </c>
       <c r="H130" s="5">
-        <v>1503.1</v>
+        <v>59.9</v>
       </c>
       <c r="I130" s="5">
-        <v>1465.7</v>
+        <v>58.9</v>
       </c>
       <c r="J130" s="5">
-        <v>1437.5</v>
+        <v>57.5</v>
       </c>
       <c r="K130" s="5">
-        <v>1407.2</v>
+        <v>56.9</v>
       </c>
       <c r="L130" s="5">
-        <v>1365.1</v>
+        <v>55.2</v>
       </c>
       <c r="M130" s="5">
-        <v>1330.2</v>
-      </c>
-      <c r="N130" s="5">
-        <v>1272.5999999999999</v>
+        <v>53.9</v>
+      </c>
+      <c r="N130" s="6">
+        <v>54</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B131" s="5">
-        <v>244.6</v>
-      </c>
-      <c r="C131" s="5">
-        <v>241.5</v>
+        <v>3.1</v>
+      </c>
+      <c r="C131" s="6">
+        <v>3</v>
       </c>
       <c r="D131" s="5">
-        <v>259.60000000000002</v>
+        <v>3.6</v>
       </c>
       <c r="E131" s="5">
-        <v>253.4</v>
+        <v>3.8</v>
       </c>
       <c r="F131" s="5">
-        <v>238.3</v>
+        <v>2.4</v>
       </c>
       <c r="G131" s="5">
-        <v>226.9</v>
-      </c>
-      <c r="H131" s="5">
-        <v>210.2</v>
+        <v>2.6</v>
+      </c>
+      <c r="H131" s="6">
+        <v>2</v>
       </c>
       <c r="I131" s="5">
-        <v>209.9</v>
+        <v>0.8</v>
       </c>
       <c r="J131" s="5">
-        <v>203.7</v>
+        <v>0.8</v>
       </c>
       <c r="K131" s="5">
-        <v>200.2</v>
+        <v>0.8</v>
       </c>
       <c r="L131" s="5">
-        <v>191.2</v>
+        <v>0.8</v>
       </c>
       <c r="M131" s="5">
-        <v>180.5</v>
+        <v>0.8</v>
       </c>
       <c r="N131" s="5">
-        <v>138.19999999999999</v>
-      </c>
-    </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A132" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B132" s="5">
-        <v>711.8</v>
-      </c>
-      <c r="C132" s="5">
-        <v>708.9</v>
-      </c>
-      <c r="D132" s="5">
-        <v>660.5</v>
-      </c>
-      <c r="E132" s="5">
-        <v>621.79999999999995</v>
-      </c>
-      <c r="F132" s="5">
-        <v>626.79999999999995</v>
-      </c>
-      <c r="G132" s="5">
-        <v>652.29999999999995</v>
-      </c>
-      <c r="H132" s="5">
-        <v>620.9</v>
-      </c>
-      <c r="I132" s="5">
-        <v>595.4</v>
-      </c>
-      <c r="J132" s="5">
-        <v>580.79999999999995</v>
-      </c>
-      <c r="K132" s="6">
-        <v>570</v>
-      </c>
-      <c r="L132" s="5">
-        <v>557.4</v>
-      </c>
-      <c r="M132" s="5">
-        <v>570.6</v>
-      </c>
-      <c r="N132" s="5">
-        <v>552.9</v>
-      </c>
-    </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A133" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B133" s="5">
-        <v>19.8</v>
-      </c>
-      <c r="C133" s="5">
-        <v>19.7</v>
-      </c>
-      <c r="D133" s="5">
-        <v>21.2</v>
-      </c>
-      <c r="E133" s="5">
-        <v>22.2</v>
-      </c>
-      <c r="F133" s="5">
-        <v>23.8</v>
-      </c>
-      <c r="G133" s="5">
-        <v>24.1</v>
-      </c>
-      <c r="H133" s="6">
-        <v>24</v>
-      </c>
-      <c r="I133" s="5">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="J133" s="5">
-        <v>22.6</v>
-      </c>
-      <c r="K133" s="5">
-        <v>26.1</v>
-      </c>
-      <c r="L133" s="5">
-        <v>29.8</v>
-      </c>
-      <c r="M133" s="5">
-        <v>33.1</v>
-      </c>
-      <c r="N133" s="5">
-        <v>35.6</v>
-      </c>
-    </row>
-    <row r="137" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A137" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C137" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D137" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E137" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F137" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G137" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H137" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I137" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J137" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K137" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L137" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M137" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N137" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A138" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B138" s="5">
-        <v>1741.5</v>
-      </c>
-      <c r="C138" s="5">
-        <v>1638.3</v>
-      </c>
-      <c r="D138" s="5">
-        <v>1482.4</v>
-      </c>
-      <c r="E138" s="5">
-        <v>1479.5</v>
-      </c>
-      <c r="F138" s="5">
-        <v>1438.5</v>
-      </c>
-      <c r="G138" s="5">
-        <v>1360.2</v>
-      </c>
-      <c r="H138" s="5">
-        <v>1340.4</v>
-      </c>
-      <c r="I138" s="5">
-        <v>1355.1</v>
-      </c>
-      <c r="J138" s="5">
-        <v>1311.7</v>
-      </c>
-      <c r="K138" s="5">
-        <v>1126.2</v>
-      </c>
-      <c r="L138" s="5">
-        <v>1183.9000000000001</v>
-      </c>
-      <c r="M138" s="5">
-        <v>1128.4000000000001</v>
-      </c>
-      <c r="N138" s="5">
-        <v>867.9</v>
-      </c>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A139" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B139" s="5">
-        <v>1562.7</v>
-      </c>
-      <c r="C139" s="5">
-        <v>1479.5</v>
-      </c>
-      <c r="D139" s="6">
-        <v>1325</v>
-      </c>
-      <c r="E139" s="5">
-        <v>1321.5</v>
-      </c>
-      <c r="F139" s="5">
-        <v>1278.4000000000001</v>
-      </c>
-      <c r="G139" s="5">
-        <v>1193.5</v>
-      </c>
-      <c r="H139" s="5">
-        <v>1176.0999999999999</v>
-      </c>
-      <c r="I139" s="5">
-        <v>1192.7</v>
-      </c>
-      <c r="J139" s="5">
-        <v>1145.9000000000001</v>
-      </c>
-      <c r="K139" s="6">
-        <v>966</v>
-      </c>
-      <c r="L139" s="5">
-        <v>1019.7</v>
-      </c>
-      <c r="M139" s="5">
-        <v>974.5</v>
-      </c>
-      <c r="N139" s="5">
-        <v>726.4</v>
-      </c>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A140" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B140" s="5">
-        <v>100.6</v>
-      </c>
-      <c r="C140" s="5">
-        <v>77.5</v>
-      </c>
-      <c r="D140" s="5">
-        <v>87.8</v>
-      </c>
-      <c r="E140" s="5">
-        <v>87.6</v>
-      </c>
-      <c r="F140" s="5">
-        <v>88.5</v>
-      </c>
-      <c r="G140" s="5">
-        <v>92.1</v>
-      </c>
-      <c r="H140" s="5">
-        <v>88.2</v>
-      </c>
-      <c r="I140" s="5">
-        <v>85.3</v>
-      </c>
-      <c r="J140" s="5">
-        <v>89.3</v>
-      </c>
-      <c r="K140" s="5">
-        <v>82.5</v>
-      </c>
-      <c r="L140" s="5">
-        <v>82.4</v>
-      </c>
-      <c r="M140" s="5">
-        <v>78.3</v>
-      </c>
-      <c r="N140" s="5">
-        <v>72.900000000000006</v>
-      </c>
-    </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A141" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B141" s="5">
-        <v>3.1</v>
-      </c>
-      <c r="C141" s="6">
-        <v>2</v>
-      </c>
-      <c r="D141" s="5">
-        <v>2.7</v>
-      </c>
-      <c r="E141" s="5">
-        <v>2.8</v>
-      </c>
-      <c r="F141" s="5">
-        <v>6.9</v>
-      </c>
-      <c r="G141" s="5">
-        <v>11.2</v>
-      </c>
-      <c r="H141" s="5">
-        <v>14.3</v>
-      </c>
-      <c r="I141" s="5">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="J141" s="5">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="K141" s="6">
-        <v>20</v>
-      </c>
-      <c r="L141" s="5">
-        <v>25.9</v>
-      </c>
-      <c r="M141" s="5">
-        <v>20.8</v>
-      </c>
-      <c r="N141" s="5">
-        <v>13.7</v>
-      </c>
-    </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A142" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B142" s="6">
-        <v>72</v>
-      </c>
-      <c r="C142" s="5">
-        <v>76.2</v>
-      </c>
-      <c r="D142" s="5">
-        <v>63.3</v>
-      </c>
-      <c r="E142" s="5">
-        <v>63.7</v>
-      </c>
-      <c r="F142" s="5">
-        <v>62.2</v>
-      </c>
-      <c r="G142" s="5">
-        <v>60.9</v>
-      </c>
-      <c r="H142" s="5">
-        <v>59.9</v>
-      </c>
-      <c r="I142" s="5">
-        <v>58.9</v>
-      </c>
-      <c r="J142" s="5">
-        <v>57.5</v>
-      </c>
-      <c r="K142" s="5">
-        <v>56.9</v>
-      </c>
-      <c r="L142" s="5">
-        <v>55.2</v>
-      </c>
-      <c r="M142" s="5">
-        <v>53.9</v>
-      </c>
-      <c r="N142" s="6">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A143" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B143" s="5">
-        <v>3.1</v>
-      </c>
-      <c r="C143" s="6">
-        <v>3</v>
-      </c>
-      <c r="D143" s="5">
-        <v>3.6</v>
-      </c>
-      <c r="E143" s="5">
-        <v>3.8</v>
-      </c>
-      <c r="F143" s="5">
-        <v>2.4</v>
-      </c>
-      <c r="G143" s="5">
-        <v>2.6</v>
-      </c>
-      <c r="H143" s="6">
-        <v>2</v>
-      </c>
-      <c r="I143" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="J143" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="K143" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="L143" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="M143" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="N143" s="5">
         <v>0.8</v>
       </c>
     </row>

</xml_diff>